<commit_message>
Labs timetable generator code changed
</commit_message>
<xml_diff>
--- a/TimeTables/CSE_Sem_5.xlsx
+++ b/TimeTables/CSE_Sem_5.xlsx
@@ -766,11 +766,31 @@
     </row>
     <row r="10" ht="15.6" customHeight="1" s="23">
       <c r="A10" s="14" t="n"/>
-      <c r="B10" s="2" t="n"/>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="n"/>
-      <c r="E10" s="2" t="n"/>
-      <c r="F10" s="10" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>SEMP - 1</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>SEMP TUT - 1</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="F10" s="10" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="16.2" customHeight="1" s="23" thickBot="1">
       <c r="A11" s="15" t="n"/>
@@ -794,13 +814,29 @@
     </row>
     <row r="13" ht="15.6" customHeight="1" s="23">
       <c r="A13" s="14" t="n"/>
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="n"/>
-      <c r="D13" s="1" t="n"/>
-      <c r="E13" s="1" t="n"/>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>SEMP - 1</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>SEMP TUT - 1</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
       <c r="F13" s="5" t="inlineStr">
         <is>
-          <t>SEMP TUT - 1</t>
+          <t>AI</t>
         </is>
       </c>
     </row>
@@ -862,21 +898,29 @@
     </row>
     <row r="19" ht="15.6" customHeight="1" s="23">
       <c r="A19" s="14" t="n"/>
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>AI LAB</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>DBMS LAB</t>
+        </is>
+      </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>DBMS</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>DBMS</t>
         </is>
       </c>
       <c r="F19" s="5" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>DBMS</t>
         </is>
       </c>
     </row>
@@ -902,21 +946,29 @@
     </row>
     <row r="22" ht="15.6" customHeight="1" s="23">
       <c r="A22" s="14" t="n"/>
-      <c r="B22" s="2" t="n"/>
-      <c r="C22" s="2" t="n"/>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>CN LAB</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F22" s="10" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>CO</t>
         </is>
       </c>
     </row>
@@ -942,21 +994,29 @@
     </row>
     <row r="25" ht="15.6" customHeight="1" s="23">
       <c r="A25" s="14" t="n"/>
-      <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>DBMS</t>
+          <t>PSE</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>DBMS</t>
+          <t>PSE</t>
         </is>
       </c>
       <c r="F25" s="5" t="inlineStr">
         <is>
-          <t>DBMS</t>
+          <t>PSE</t>
         </is>
       </c>
     </row>

</xml_diff>